<commit_message>
change content file thuc hanh git.xlsx
</commit_message>
<xml_diff>
--- a/git_learn/thuc hanh git.xlsx
+++ b/git_learn/thuc hanh git.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t xml:space="preserve">Câu lệnh</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Cấu hình email</t>
   </si>
   <si>
-    <t xml:space="preserve">Tạo file index.html</t>
+    <t xml:space="preserve">tạo file “thuc hanh git.xlsx” trong thư mục git_learn</t>
   </si>
   <si>
     <t xml:space="preserve">git status</t>
@@ -70,16 +70,16 @@
     <t xml:space="preserve">    + Staging Area: khu vuc co the theo doi duoc cac file se duoc thuc hien cac lan commit tiep theo =&gt; se duoc dua vao trong git repo voi noi dung la nhung thay doi tren file</t>
   </si>
   <si>
-    <t xml:space="preserve">git add index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thực hiện đưa file index.html sang khu vực Staging Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra trạng thái file index.html đã được add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git commit -m “add index.html file”</t>
+    <t xml:space="preserve">git add .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thực hiện đưa các file sang khu vực Staging Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra trạng thái file đã được add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m “add file thuc hanh git.xlxs ”</t>
   </si>
   <si>
     <t xml:space="preserve">Thực hiện ghi vao kho chung cac thay doi =&gt; cac file trong Staging Area se chuyen sang trang thai Commited</t>
@@ -134,18 +134,6 @@
     <t xml:space="preserve">Refresh trình duyệt để update thay đổi</t>
   </si>
   <si>
-    <t xml:space="preserve">Thêm các folder, file mới</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Thêm folder css: chứa các file css</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Thêm folder js: chứa các file JavaScript</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- folder fontawesome-free-6.1.2: các các design icon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tạo branch mới để tránh ảnh hưởng đến branch chính(master)</t>
   </si>
   <si>
@@ -173,9 +161,6 @@
     <t xml:space="preserve">Folder fontawesome-free-6.1.2 không còn trong Untracked files</t>
   </si>
   <si>
-    <t xml:space="preserve">git add .</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thực hiện chuyển tất cả các file sang trạng thái Staging Area chờ thực hiện commit</t>
   </si>
   <si>
@@ -228,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve">Thực hiện commit file myScript.js với nội dung “update myScript file in folder”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git add index.html</t>
   </si>
   <si>
     <t xml:space="preserve">Chuyển file index.html sang Staging Area</t>
@@ -381,19 +369,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>453240</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>410760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -402,44 +390,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="250200"/>
-          <a:ext cx="8150040" cy="1328400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>410400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6605640" y="2115360"/>
+          <a:off x="6606000" y="2115720"/>
           <a:ext cx="7293240" cy="1299960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -455,29 +406,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>20160</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>270720</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>513000</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 3" descr=""/>
+        <xdr:cNvPr id="1" name="Image 9" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="3980160"/>
-          <a:ext cx="12038040" cy="6501960"/>
+          <a:off x="6625800" y="29821680"/>
+          <a:ext cx="5747400" cy="1299960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,398 +443,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>729360</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26640</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 4" descr=""/>
+        <xdr:cNvPr id="2" name="Image 15" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="12403440"/>
-          <a:ext cx="10868400" cy="6712200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>677160</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6605640" y="20404440"/>
-          <a:ext cx="7560000" cy="3011400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>174600</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 6" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6605640" y="24364800"/>
-          <a:ext cx="6243480" cy="1682280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 7" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6616080" y="27564120"/>
-          <a:ext cx="7719480" cy="1605960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>512640</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 9" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6625440" y="29905200"/>
-          <a:ext cx="5747400" cy="1299960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3911040</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
-      <xdr:row>172</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 10" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6586200" y="32164200"/>
-          <a:ext cx="8242920" cy="2514240"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>49680</xdr:colOff>
-      <xdr:row>178</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>792360</xdr:colOff>
-      <xdr:row>192</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 11" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6655320" y="35715600"/>
-          <a:ext cx="9253800" cy="2657520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
-      <xdr:row>200</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>670320</xdr:colOff>
-      <xdr:row>229</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 12" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6615720" y="40041000"/>
-          <a:ext cx="10799280" cy="5450040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3921480</xdr:colOff>
-      <xdr:row>238</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>86040</xdr:colOff>
-      <xdr:row>244</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 13" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6596640" y="47401560"/>
-          <a:ext cx="6163920" cy="1443240"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>249</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>524160</xdr:colOff>
-      <xdr:row>252</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 14" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6605640" y="49787640"/>
-          <a:ext cx="4964760" cy="687960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>254</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>26280</xdr:colOff>
-      <xdr:row>267</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 15" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6605640" y="50740200"/>
+          <a:off x="6606000" y="50433120"/>
           <a:ext cx="6095160" cy="2610000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -899,28 +480,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>271</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>115560</xdr:colOff>
+      <xdr:colOff>115920</xdr:colOff>
       <xdr:row>281</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 16" descr=""/>
+        <xdr:cNvPr id="3" name="Image 16" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="53978760"/>
+          <a:off x="6606000" y="53671320"/>
           <a:ext cx="6184440" cy="2304000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -936,28 +517,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>286</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>402120</xdr:colOff>
+      <xdr:colOff>402480</xdr:colOff>
       <xdr:row>298</xdr:row>
       <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Image 17" descr=""/>
+        <xdr:cNvPr id="4" name="Image 17" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="57148200"/>
+          <a:off x="6606000" y="56841120"/>
           <a:ext cx="6471000" cy="2504520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -973,28 +554,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>303</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>346320</xdr:colOff>
+      <xdr:colOff>346680</xdr:colOff>
       <xdr:row>312</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Image 18" descr=""/>
+        <xdr:cNvPr id="5" name="Image 18" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <a:blip r:embed="rId6"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="60537240"/>
+          <a:off x="6606000" y="60230160"/>
           <a:ext cx="4786920" cy="1892520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1010,28 +591,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>316</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>384120</xdr:colOff>
+      <xdr:colOff>384480</xdr:colOff>
       <xdr:row>322</xdr:row>
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Image 19" descr=""/>
+        <xdr:cNvPr id="6" name="Image 19" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <a:blip r:embed="rId7"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="63164160"/>
+          <a:off x="6606000" y="62857080"/>
           <a:ext cx="5638680" cy="1510200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1047,28 +628,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>327</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>174600</xdr:colOff>
+      <xdr:colOff>174960</xdr:colOff>
       <xdr:row>336</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Image 20" descr=""/>
+        <xdr:cNvPr id="7" name="Image 20" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <a:blip r:embed="rId8"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="65560680"/>
+          <a:off x="6606000" y="65253600"/>
           <a:ext cx="6243480" cy="1883160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1084,28 +665,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>340</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>153360</xdr:colOff>
       <xdr:row>348</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Image 21" descr=""/>
+        <xdr:cNvPr id="8" name="Image 21" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
+        <a:blip r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="68037120"/>
+          <a:off x="6606000" y="67730040"/>
           <a:ext cx="7035840" cy="1682280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1121,28 +702,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>352</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>121680</xdr:colOff>
+      <xdr:colOff>122040</xdr:colOff>
       <xdr:row>365</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Image 22" descr=""/>
+        <xdr:cNvPr id="9" name="Image 22" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
+        <a:blip r:embed="rId10"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="70473600"/>
+          <a:off x="6606000" y="70166520"/>
           <a:ext cx="7818480" cy="2696040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1158,28 +739,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>370</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>377</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Image 23" descr=""/>
+        <xdr:cNvPr id="10" name="Image 23" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
+        <a:blip r:embed="rId11"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="74053080"/>
+          <a:off x="6606000" y="73746000"/>
           <a:ext cx="5589000" cy="1414440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1195,28 +776,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>380</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>534960</xdr:colOff>
-      <xdr:row>393</xdr:row>
-      <xdr:rowOff>191160</xdr:rowOff>
+      <xdr:colOff>535320</xdr:colOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 24" descr=""/>
+        <xdr:cNvPr id="11" name="Image 24" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
+        <a:blip r:embed="rId12"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="75958200"/>
+          <a:off x="6606000" y="75651120"/>
           <a:ext cx="9046080" cy="2667240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1232,28 +813,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>398</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>623880</xdr:colOff>
+      <xdr:colOff>624240</xdr:colOff>
       <xdr:row>409</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Image 25" descr=""/>
+        <xdr:cNvPr id="12" name="Image 25" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
+        <a:blip r:embed="rId13"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="79387200"/>
+          <a:off x="6606000" y="79080120"/>
           <a:ext cx="9135000" cy="2227320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1269,28 +850,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>413</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>421</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Image 26" descr=""/>
+        <xdr:cNvPr id="13" name="Image 26" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
+        <a:blip r:embed="rId14"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="82244520"/>
+          <a:off x="6606000" y="81937080"/>
           <a:ext cx="6164640" cy="1682280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1306,28 +887,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>425</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>202680</xdr:colOff>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>427</xdr:row>
       <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Image 27" descr=""/>
+        <xdr:cNvPr id="14" name="Image 27" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
+        <a:blip r:embed="rId15"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="84681000"/>
+          <a:off x="6606000" y="84373560"/>
           <a:ext cx="7085520" cy="630360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1343,28 +924,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>430</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>477720</xdr:colOff>
+      <xdr:colOff>478080</xdr:colOff>
       <xdr:row>432</xdr:row>
       <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Image 28" descr=""/>
+        <xdr:cNvPr id="15" name="Image 28" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
+        <a:blip r:embed="rId16"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="85784040"/>
+          <a:off x="6606000" y="85476600"/>
           <a:ext cx="8174520" cy="621000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1380,28 +961,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>435</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>105840</xdr:colOff>
       <xdr:row>456</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Image 29" descr=""/>
+        <xdr:cNvPr id="16" name="Image 29" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28"/>
+        <a:blip r:embed="rId17"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="86887080"/>
+          <a:off x="6606000" y="86580000"/>
           <a:ext cx="6174360" cy="4149360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1417,28 +998,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>462</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>342720</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>469</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Image 30" descr=""/>
+        <xdr:cNvPr id="17" name="Image 30" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29"/>
+        <a:blip r:embed="rId18"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="92030400"/>
+          <a:off x="6606000" y="91723320"/>
           <a:ext cx="6411600" cy="1376280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1454,28 +1035,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>472</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>473040</xdr:colOff>
+      <xdr:colOff>473400</xdr:colOff>
       <xdr:row>479</xdr:row>
       <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Image 31" descr=""/>
+        <xdr:cNvPr id="18" name="Image 31" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30"/>
+        <a:blip r:embed="rId19"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="93935520"/>
+          <a:off x="6606000" y="93628080"/>
           <a:ext cx="5727600" cy="1548360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1491,28 +1072,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>483</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>782280</xdr:colOff>
+      <xdr:colOff>782640</xdr:colOff>
       <xdr:row>500</xdr:row>
       <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Image 32" descr=""/>
+        <xdr:cNvPr id="19" name="Image 32" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31"/>
+        <a:blip r:embed="rId20"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="96181560"/>
+          <a:off x="6606000" y="95874480"/>
           <a:ext cx="9293400" cy="3394080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1528,29 +1109,325 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>505</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>525600</xdr:colOff>
       <xdr:row>520</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Image 33" descr=""/>
+        <xdr:cNvPr id="20" name="Image 33" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32"/>
+        <a:blip r:embed="rId21"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605640" y="100372680"/>
+          <a:off x="6606000" y="100065600"/>
           <a:ext cx="9036360" cy="2638440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>29160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>240480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>439920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId22"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6634800" y="240480"/>
+          <a:ext cx="7293600" cy="1665360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10080</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>150120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>391680</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>14760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId23"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6615720" y="4320720"/>
+          <a:ext cx="7264440" cy="4818960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342360</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>52200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId24"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6605640" y="10077120"/>
+          <a:ext cx="7225200" cy="1316520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352080</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>180360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId25"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6605640" y="27480240"/>
+          <a:ext cx="7234920" cy="3950280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381600</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId26"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6605640" y="32232600"/>
+          <a:ext cx="7264440" cy="4389120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>618480</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>39960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId27"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6605640" y="37335960"/>
+          <a:ext cx="9129600" cy="2242080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>550800</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>172080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId28"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="40188240"/>
+          <a:ext cx="7156440" cy="1154520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>194760</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>82440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Image 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId29"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6605640" y="47111760"/>
+          <a:ext cx="7077600" cy="1526400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1572,8 +1449,8 @@
   </sheetPr>
   <dimension ref="A1:C524"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C525" activeCellId="0" sqref="C525"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A290" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A252" activeCellId="0" sqref="A252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1671,7 +1548,6 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,20 +1601,32 @@
       <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
@@ -1804,9 +1692,13 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+    <row r="48" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
@@ -1860,22 +1752,6 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
@@ -2032,13 +1908,8 @@
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>20</v>
-      </c>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2"/>
@@ -2115,14 +1986,6 @@
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
-    </row>
-    <row r="123" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2"/>
@@ -2372,9 +2235,6 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2"/>
-      <c r="B179" s="2" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2"/>
@@ -2410,7 +2270,9 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2"/>
-      <c r="B188" s="2"/>
+      <c r="B188" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2"/>
@@ -2444,49 +2306,9 @@
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
     </row>
-    <row r="197" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="2"/>
-      <c r="B197" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="2"/>
-      <c r="B198" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="2"/>
-      <c r="B199" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="2"/>
-      <c r="B200" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-    </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
-    </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2"/>
-      <c r="B204" s="2"/>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2"/>
@@ -2619,7 +2441,7 @@
     <row r="237" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2"/>
       <c r="B237" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,30 +2450,34 @@
     </row>
     <row r="239" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
     </row>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
+    <row r="241" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
     </row>
-    <row r="243" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,14 +2504,6 @@
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
     </row>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
@@ -2777,7 +2595,7 @@
     <row r="272" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2"/>
       <c r="B272" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +2673,7 @@
     <row r="290" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2"/>
       <c r="B290" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,10 +2730,10 @@
     </row>
     <row r="304" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2972,16 +2790,16 @@
     </row>
     <row r="318" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2"/>
       <c r="B319" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3021,7 +2839,7 @@
         <v>21</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,16 +2892,16 @@
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2"/>
       <c r="B342" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,10 +2950,10 @@
     </row>
     <row r="354" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,10 +3022,10 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,7 +3077,7 @@
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2"/>
       <c r="B383" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3147,7 @@
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2"/>
       <c r="B400" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,10 +3204,10 @@
     </row>
     <row r="414" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3438,10 +3256,10 @@
     </row>
     <row r="426" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3462,18 +3280,18 @@
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,7 +3311,7 @@
         <v>21</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3602,18 +3420,18 @@
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3650,7 +3468,7 @@
     </row>
     <row r="473" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B473" s="2" t="s">
         <v>35</v>
@@ -3709,7 +3527,7 @@
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2"/>
       <c r="B486" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,12 +3613,12 @@
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2"/>
       <c r="B507" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>